<commit_message>
Add alert when 30 seconds left, small ui fixes
</commit_message>
<xml_diff>
--- a/surveyapp/data/users_surveys/1lbCvs1hADW3mD5c66mzpqb7ziKmDGtr5QoGX7pISYs.xlsx
+++ b/surveyapp/data/users_surveys/1lbCvs1hADW3mD5c66mzpqb7ziKmDGtr5QoGX7pISYs.xlsx
@@ -422,15 +422,36 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2">
+        <v>1689535950035</v>
+      </c>
+      <c r="C2">
+        <v>1689536250035</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3">
+        <v>1689536281159</v>
+      </c>
+      <c r="C3">
+        <v>1689536576890</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1689536578067</v>
+      </c>
+      <c r="C4">
+        <v>1689536878067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>